<commit_message>
VerifyEmail page , setnewPassword page , resetpasswordPage
</commit_message>
<xml_diff>
--- a/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\UGapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C880731-C86C-49EB-87F8-747084AE36C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AD02757C-5B94-47D8-B9A0-721E2FC16B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +13,7 @@
     <sheet name="CreateAccountTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="HlaChI891gGz17+51dPFo8qf561pCnka8lvLU1BAhSA="/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -74,13 +70,10 @@
     <t>Testug</t>
   </si>
   <si>
-    <t>Testug@asu.edu</t>
-  </si>
-  <si>
-    <t>TEST123123123</t>
-  </si>
-  <si>
-    <t>Test12</t>
+    <t>testug@test.asu.edu</t>
+  </si>
+  <si>
+    <t>testug@asu.edu</t>
   </si>
 </sst>
 </file>
@@ -98,37 +91,34 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,15 +140,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,10 +452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -493,100 +484,80 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{829B1134-51DA-4036-841F-87975DF98B0B}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{D78C28E5-1EC6-4FFC-9475-E245F3982598}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{768486F4-5B12-4B65-8F49-667B2632A759}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{495326F2-5F66-4FE0-970B-D1157C9DF3C5}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{70F5085C-BE38-4EB3-A3DC-F3494B759FB1}"/>
-    <hyperlink ref="B5" r:id="rId6" xr:uid="{03FD5B89-D1E2-45A5-9AA2-EABA74DFBBEE}"/>
-    <hyperlink ref="B4" r:id="rId7" xr:uid="{D1088D73-B312-4478-B0A4-01AFD275AC59}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{450D01D8-C195-4412-B4A3-BBF48F5702F0}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{25E016FA-2D03-44C5-B186-5699102F8FAA}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C3E9831C-B7FE-4F7E-A83C-696EDFC5C780}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E0711331-B2A1-49E4-90B3-B05126639987}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{D1D995E1-F7FF-4ACB-B614-825B2EA5A2A3}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{608E3CD1-3B3E-407C-89A3-7049494CAEE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Used clear method instead of performKeyBoardAction method ,completed login Page,added testng class
</commit_message>
<xml_diff>
--- a/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB62307-165D-44D8-ADB9-91E12AAAA6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E911BC0-11AE-4690-8755-F08EF122E748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="108" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>testug@test.asu.edu</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Testug@1test.asu.edu</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -410,7 +416,7 @@
     <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -421,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -433,14 +439,34 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{762CACF4-C0C3-4181-A5C7-AAB3826ABC7F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -451,7 +477,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>